<commit_message>
Dictionary replace and notebook creation
</commit_message>
<xml_diff>
--- a/Lab 1 - Clustering/datos/Diccionario_BiciAlpes.xlsx
+++ b/Lab 1 - Clustering/datos/Diccionario_BiciAlpes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dell\Documents\Uniandes\Cursos_2023_10\IN\Laboratorio clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812F410E-90B5-4520-8C4B-AD02EA719510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820AFABA-2F27-46BC-A39D-538B0412B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
-    <t>numérico</t>
-  </si>
-  <si>
     <t>categórica</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>Características del cruce (No hay cruce = 0, Rotonda = 1, Minirrotonda = 2, Unión en T = 3, Carretera de acceso = 5, Encrucijada = 6, Más de cuatro salidas = 7, Entrada privada = 8, Otros cruces = 9, missign o fuera de rango = -1).</t>
+  </si>
+  <si>
+    <t>categórico</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,167 +499,167 @@
   <sheetData>
     <row r="1" spans="1:3" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sort of kmeans implemented
</commit_message>
<xml_diff>
--- a/Lab 1 - Clustering/datos/Diccionario_BiciAlpes.xlsx
+++ b/Lab 1 - Clustering/datos/Diccionario_BiciAlpes.xlsx
@@ -134,19 +134,19 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -534,7 +534,7 @@
     <col min="3" max="3" style="7" width="187.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="25.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -719,27 +719,27 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>

</xml_diff>